<commit_message>
Update timelog to use template
</commit_message>
<xml_diff>
--- a/project-planning/timelogs/Nikolas_Time_Log.xlsx
+++ b/project-planning/timelogs/Nikolas_Time_Log.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leslienk\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F3EAF6F-1F15-470E-9E67-B887F55EC507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110E54D4-A115-400B-9D5C-CFA0EE0F8EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F20C800-7844-4890-B3E4-00D090BA92A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -31,67 +28,100 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Time Log </t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Student ID / Matrikelnummer:</t>
   </si>
   <si>
     <t>Hours</t>
   </si>
   <si>
-    <t>Scrum Backlogs</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>10.10.25</t>
-  </si>
-  <si>
-    <t>16.10.25</t>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Calendar Week</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Software Projekt 2020/2021</t>
+  </si>
+  <si>
+    <t>Project
+Week</t>
+  </si>
+  <si>
+    <t>Nikolas Leslie</t>
+  </si>
+  <si>
+    <t>~1</t>
+  </si>
+  <si>
+    <t>Backlog template, planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -99,20 +129,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -125,7 +213,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-Design">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -135,44 +223,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -200,31 +288,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -252,23 +323,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,6 +384,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -338,13 +399,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -409,95 +463,385 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C7F2F3-E05A-4C39-B3AF-55AFA98B1855}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11" style="5" customWidth="1"/>
+    <col min="2" max="4" width="11.296875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="151.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="E3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6012846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B7" s="11">
+        <f>_xlfn.ISOWEEKNUM(C7)</f>
+        <v>40</v>
+      </c>
+      <c r="C7" s="6">
+        <v>44102</v>
+      </c>
+      <c r="D7" s="7">
+        <f>C7+6</f>
+        <v>44108</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B8" s="11">
+        <f t="shared" ref="B8:B22" si="0">_xlfn.ISOWEEKNUM(C8)</f>
+        <v>41</v>
+      </c>
+      <c r="C8" s="7">
+        <f>C7+7</f>
+        <v>44109</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" ref="D8:D22" si="1">C8+6</f>
+        <v>44115</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B9" s="11">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:C22" si="2">C8+7</f>
+        <v>44116</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>44122</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B10" s="11">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="2"/>
+        <v>44123</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>44129</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="2"/>
+        <v>44130</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>44136</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B12" s="11">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="2"/>
+        <v>44137</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>44143</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.52638888888888891</v>
-      </c>
-      <c r="E3" s="2">
-        <f>D3-C3</f>
-        <v>1.9444444444444486E-2</v>
-      </c>
+      <c r="B13" s="11">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="2"/>
+        <v>44144</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>44150</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>8</v>
+      </c>
+      <c r="B14" s="11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="2"/>
+        <v>44151</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>44157</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>9</v>
+      </c>
+      <c r="B15" s="11">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="2"/>
+        <v>44158</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>44164</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>10</v>
+      </c>
+      <c r="B16" s="11">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="2"/>
+        <v>44165</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>44171</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>11</v>
+      </c>
+      <c r="B17" s="11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="2"/>
+        <v>44172</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>44178</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>12</v>
+      </c>
+      <c r="B18" s="11">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="2"/>
+        <v>44179</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>44185</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>13</v>
+      </c>
+      <c r="B19" s="11">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" si="2"/>
+        <v>44186</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
+        <v>44192</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>14</v>
+      </c>
+      <c r="B20" s="11">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="2"/>
+        <v>44193</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>44199</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>15</v>
+      </c>
+      <c r="B21" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="2"/>
+        <v>44200</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
+        <v>44206</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>16</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="2"/>
+        <v>44207</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
+        <v>44213</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>